<commit_message>
Changed sound file level and tweaked instructions
</commit_message>
<xml_diff>
--- a/practice_sentences.xlsx
+++ b/practice_sentences.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpeelle/Desktop/sentence_intelligibility_2024-12/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpeelle/Library/CloudStorage/Dropbox/work/RESEARCH/experiments/sentence_intelligibility_01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F59D837-F9AE-F84A-B948-A5D6DB143548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C815F3-40E0-0744-9339-881323B85766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{CDA7BABA-58B1-874D-8D52-F30B83AD5DAB}"/>
+    <workbookView xWindow="8820" yWindow="6920" windowWidth="29660" windowHeight="11900" xr2:uid="{CDA7BABA-58B1-874D-8D52-F30B83AD5DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>audio</t>
   </si>
@@ -50,10 +50,19 @@
     <t>practice_intro_text</t>
   </si>
   <si>
-    <t>Great! Now we will practice listening to a sentence with noise. This may be more challenging, so just try your best! Press 'Return' to continue.</t>
-  </si>
-  <si>
-    <t>We will first practice listening to a sentence without noise. Press 'Return' to start the practice round.</t>
+    <t>We will first practice listening to a sentence without noise. Press 'Return' to continue.</t>
+  </si>
+  <si>
+    <t>Great! Now we will practice listening to sentences with noise. This may be more challenging, so just try your best! Press 'Return' to continue.</t>
+  </si>
+  <si>
+    <t>If you are not sure of what you hear, just do your best. Please guess if possible.</t>
+  </si>
+  <si>
+    <t>soundfiles/NU1109_0825_talker01_SNR-5.wav</t>
+  </si>
+  <si>
+    <t>soundfiles/NU1109_0792_talker01_SNR-5.wav</t>
   </si>
 </sst>
 </file>
@@ -425,16 +434,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FBD4332-2999-234B-924A-C1B3F4DAAD6C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="94.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.83203125" customWidth="1"/>
+    <col min="1" max="1" width="150" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -447,7 +456,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -455,10 +464,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>